<commit_message>
fix validation upload gambar
</commit_message>
<xml_diff>
--- a/public/excel/group/bts.xlsx
+++ b/public/excel/group/bts.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>d_kelas</t>
   </si>
@@ -46,31 +46,34 @@
     <t>nama</t>
   </si>
   <si>
-    <t>no system is safe</t>
-  </si>
-  <si>
     <t>Si_A.jpg</t>
   </si>
   <si>
     <t>Si_B.jpg</t>
   </si>
   <si>
-    <t>ah boong kali lu A</t>
-  </si>
-  <si>
-    <t>TET</t>
-  </si>
-  <si>
     <t>nis</t>
   </si>
   <si>
-    <t>Martha</t>
-  </si>
-  <si>
-    <t>Koko</t>
-  </si>
-  <si>
     <t>TKJ</t>
+  </si>
+  <si>
+    <t>not error</t>
+  </si>
+  <si>
+    <t>tei</t>
+  </si>
+  <si>
+    <t>Si_C.jpg</t>
+  </si>
+  <si>
+    <t>si_D.jpg</t>
+  </si>
+  <si>
+    <t>ah masa</t>
+  </si>
+  <si>
+    <t>tbsm</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -438,7 +441,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -458,19 +461,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>192010235</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -478,21 +481,61 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>192010036</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3">
+      <c r="F5">
         <v>4</v>
       </c>
     </row>

</xml_diff>